<commit_message>
fixed update counts and added sync to RenderTask.Run;
</commit_message>
<xml_diff>
--- a/src/TrafoUpdatePerformance.xlsx
+++ b/src/TrafoUpdatePerformance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Initial</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>correct again (initial execution)</t>
+  </si>
+  <si>
+    <t>always hashset</t>
+  </si>
+  <si>
+    <t>VolaileCollection using C# List</t>
   </si>
 </sst>
 </file>
@@ -127,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -135,6 +141,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,7 +153,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -169,9 +176,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Initial</c:v>
                 </c:pt>
@@ -225,16 +232,22 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>evaluate inline</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>always hashset</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>VolaileCollection using C# List</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$19</c:f>
+              <c:f>Sheet1!$B$2:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>2.63</c:v>
                 </c:pt>
@@ -287,7 +300,13 @@
                   <c:v>11.069552669552671</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.525829725829727</c:v>
+                  <c:v>21.97</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.99</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -309,9 +328,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Initial</c:v>
                 </c:pt>
@@ -365,16 +384,22 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>evaluate inline</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>always hashset</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>VolaileCollection using C# List</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$19</c:f>
+              <c:f>Sheet1!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>2.1192906976744186</c:v>
                 </c:pt>
@@ -428,29 +453,35 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>16.54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18.813591260810195</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.673117888029132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="52009216"/>
-        <c:axId val="58597376"/>
+        <c:axId val="71071616"/>
+        <c:axId val="71073152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52009216"/>
+        <c:axId val="71071616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58597376"/>
+        <c:crossAx val="71073152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58597376"/>
+        <c:axId val="71073152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,7 +489,365 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52009216"/>
+        <c:crossAx val="71071616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Monster64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Initial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>eval depth instead of eval-stack</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>merged depth and locking try-finally</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>no telemetry</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>no List.iter in ChangeableResource UpdateCPU</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>No DirtySet in UniformBuffer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Correct again with Sync (possibly bad)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VolatileSet remains HashSet when consumed</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>no lock in VolatileCollection</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DuplicatePriorityQueue local mutable for outs</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>using null as none-value for current obj in Transaction</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>NativePtr write instead of Marshal.StructureToPtr</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>IWriter</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>optimized update-counting</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>TrafoMultiplyMod</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>UniformBufferView</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>correct again (initial execution)</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>evaluate inline</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>always hashset</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>VolaileCollection using C# List</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5209125475285079E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.7453183520598232E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50375939849624052</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32432432432432412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-6.9727891156462607E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6782449725776969E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1884550084889645E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8657718120805438E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.1999999999999806E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.6548956661315977E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6871165644171793E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.28205128205128216</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1764705882352899E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3073593073593075</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.5452538631346435E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.98472338095734657</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.13746017296313151</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.8839535814325918E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mobile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Initial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>eval depth instead of eval-stack</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>merged depth and locking try-finally</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>no telemetry</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>no List.iter in ChangeableResource UpdateCPU</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>No DirtySet in UniformBuffer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Correct again with Sync (possibly bad)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VolatileSet remains HashSet when consumed</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>no lock in VolatileCollection</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DuplicatePriorityQueue local mutable for outs</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>using null as none-value for current obj in Transaction</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>NativePtr write instead of Marshal.StructureToPtr</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>IWriter</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>optimized update-counting</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>TrafoMultiplyMod</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>UniformBufferView</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>correct again (initial execution)</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>evaluate inline</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>always hashset</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>VolaileCollection using C# List</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5209125475285301E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.7453183520599342E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50375939849624052</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32432432432432412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-6.9727891156462496E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6782449725776747E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1884550084889645E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.865771812080566E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.1999999999999806E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.6548956661315977E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6871165644171793E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.28205128205128216</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1764705882352899E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3073593073593075</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.5452538631346657E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85426008968609857</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.13746017296313151</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.8839535814325918E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="162368128"/>
+        <c:axId val="162578816"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="162368128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="162578816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="162578816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="162368128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -482,15 +871,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>942974</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>742949</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -504,6 +893,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723899</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -797,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -809,10 +1228,13 @@
     <col min="2" max="3" width="10.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" style="2" customWidth="1"/>
-    <col min="7" max="22" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="5" customWidth="1"/>
+    <col min="10" max="22" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
@@ -825,8 +1247,14 @@
       <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -844,11 +1272,14 @@
         <f t="shared" ref="F2:F14" si="1">E2*F$16/E$16</f>
         <v>210.88530374999999</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -866,8 +1297,16 @@
         <f t="shared" si="1"/>
         <v>210.93582125</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3" s="5">
+        <f>(B3/B2 - 1)</f>
+        <v>1.5209125475285079E-2</v>
+      </c>
+      <c r="I3" s="5">
+        <f>(C3/C2 - 1)</f>
+        <v>1.5209125475285301E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -885,8 +1324,16 @@
         <f t="shared" si="1"/>
         <v>210.48958333333334</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="5">
+        <f>(B4/B3 - 1)</f>
+        <v>-3.7453183520598232E-3</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" ref="I4:I19" si="2">(C4/C3 - 1)</f>
+        <v>-3.7453183520599342E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -904,8 +1351,16 @@
         <f t="shared" si="1"/>
         <v>207.68586208333332</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="H5" s="5">
+        <f>(B5/B4 - 1)</f>
+        <v>0.50375939849624052</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="2"/>
+        <v>0.50375939849624052</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -923,8 +1378,16 @@
         <f t="shared" si="1"/>
         <v>197.43080958333334</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="H6" s="5">
+        <f>(B6/B5 - 1)</f>
+        <v>0.1100000000000001</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="2"/>
+        <v>0.1100000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -942,8 +1405,16 @@
         <f t="shared" si="1"/>
         <v>197.01824999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="H7" s="5">
+        <f>(B7/B6 - 1)</f>
+        <v>0.32432432432432412</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="2"/>
+        <v>0.32432432432432412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -961,8 +1432,16 @@
         <f t="shared" si="1"/>
         <v>205.55570749999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="H8" s="5">
+        <f>(B8/B7 - 1)</f>
+        <v>-6.9727891156462607E-2</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="2"/>
+        <v>-6.9727891156462496E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -980,8 +1459,16 @@
         <f t="shared" si="1"/>
         <v>197.01824999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="H9" s="5">
+        <f>(B9/B8 - 1)</f>
+        <v>7.6782449725776969E-2</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="2"/>
+        <v>7.6782449725776747E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -999,8 +1486,16 @@
         <f t="shared" si="1"/>
         <v>207.30698083333334</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10" s="5">
+        <f>(B10/B9 - 1)</f>
+        <v>1.1884550084889645E-2</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="2"/>
+        <v>1.1884550084889645E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1018,8 +1513,19 @@
         <f t="shared" si="1"/>
         <v>208.51098124999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="H11" s="5">
+        <f>(B11/B10 - 1)</f>
+        <v>4.8657718120805438E-2</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="2"/>
+        <v>4.865771812080566E-2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1037,8 +1543,16 @@
         <f t="shared" si="1"/>
         <v>206.27979166666668</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="H12" s="5">
+        <f>(B12/B11 - 1)</f>
+        <v>-3.1999999999999806E-3</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="2"/>
+        <v>-3.1999999999999806E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1056,8 +1570,16 @@
         <f t="shared" si="1"/>
         <v>203.4929095833333</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="H13" s="5">
+        <f>(B13/B12 - 1)</f>
+        <v>4.6548956661315977E-2</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="2"/>
+        <v>4.6548956661315977E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1075,8 +1597,16 @@
         <f t="shared" si="1"/>
         <v>193.65041666666667</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="H14" s="5">
+        <f>(B14/B13 - 1)</f>
+        <v>1.6871165644171793E-2</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="2"/>
+        <v>1.6871165644171793E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1094,8 +1624,16 @@
         <f>E15*F$16/E$16</f>
         <v>202.69304916666667</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="H15" s="5">
+        <f>(B15/B14 - 1)</f>
+        <v>0.28205128205128216</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" si="2"/>
+        <v>0.28205128205128216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1111,8 +1649,16 @@
       <c r="F16" s="4">
         <v>202.07</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="H16" s="5">
+        <f>(B16/B15 - 1)</f>
+        <v>1.1764705882352899E-2</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" si="2"/>
+        <v>1.1764705882352899E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1130,8 +1676,16 @@
       <c r="F17" s="4">
         <v>458.58</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="H17" s="5">
+        <f>(B17/B16 - 1)</f>
+        <v>0.3073593073593075</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.3073593073593075</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1150,24 +1704,92 @@
       <c r="F18" s="2">
         <v>465.19</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="H18" s="5">
+        <f>(B18/B17 - 1)</f>
+        <v>-1.5452538631346435E-2</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" si="2"/>
+        <v>-1.5452538631346657E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="3">
-        <f>C19*B$16/C$16</f>
-        <v>20.525829725829727</v>
+      <c r="B19" s="4">
+        <v>21.97</v>
       </c>
       <c r="C19" s="2">
         <v>16.54</v>
       </c>
-      <c r="E19" s="3">
-        <f>F19*E$16/F$16</f>
-        <v>556.90404315336264</v>
+      <c r="E19" s="4">
+        <v>494</v>
       </c>
       <c r="F19" s="2">
         <v>468.89</v>
+      </c>
+      <c r="H19" s="5">
+        <f>(B19/B18 - 1)</f>
+        <v>0.98472338095734657</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" si="2"/>
+        <v>0.85426008968609857</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
+        <v>24.99</v>
+      </c>
+      <c r="C20" s="3">
+        <f>B20*C$19/B$19</f>
+        <v>18.813591260810195</v>
+      </c>
+      <c r="E20" s="2">
+        <v>462</v>
+      </c>
+      <c r="F20" s="3">
+        <f>E20*F$19/E$19</f>
+        <v>438.51655870445342</v>
+      </c>
+      <c r="H20" s="5">
+        <f>(B20/B19 - 1)</f>
+        <v>0.13746017296313151</v>
+      </c>
+      <c r="I20" s="5">
+        <f t="shared" ref="I20" si="3">(C20/C19 - 1)</f>
+        <v>0.13746017296313151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="2">
+        <v>27.46</v>
+      </c>
+      <c r="C21" s="3">
+        <f>B21*C$19/B$19</f>
+        <v>20.673117888029132</v>
+      </c>
+      <c r="E21" s="2">
+        <v>462</v>
+      </c>
+      <c r="F21" s="3">
+        <f>E21*F$19/E$19</f>
+        <v>438.51655870445342</v>
+      </c>
+      <c r="H21" s="5">
+        <f>(B21/B20 - 1)</f>
+        <v>9.8839535814325918E-2</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" ref="I21" si="4">(C21/C20 - 1)</f>
+        <v>9.8839535814325918E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some refactoring (moved conversion stuff to its own file)
</commit_message>
<xml_diff>
--- a/src/TrafoUpdatePerformance.xlsx
+++ b/src/TrafoUpdatePerformance.xlsx
@@ -1216,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1234,7 +1234,7 @@
     <col min="10" max="22" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>1.5209125475285301E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>-3.7453183520599342E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>0.50375939849624052</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>0.1100000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>0.32432432432432412</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>-6.9727891156462496E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>7.6782449725776747E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>1.1884550084889645E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>-3.1999999999999806E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1578,8 +1578,12 @@
         <f t="shared" si="2"/>
         <v>4.6548956661315977E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="M13">
+        <f t="shared" ref="M13:M20" si="3">(E13*15625)/60</f>
+        <v>62940.104166666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1605,8 +1609,12 @@
         <f t="shared" si="2"/>
         <v>1.6871165644171793E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>59895.833333333336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1632,8 +1640,12 @@
         <f t="shared" si="2"/>
         <v>0.28205128205128216</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>62692.708333333336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1657,8 +1669,12 @@
         <f t="shared" si="2"/>
         <v>1.1764705882352899E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="M16">
+        <f>(E16*15625)/60</f>
+        <v>62500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1684,8 +1700,12 @@
         <f t="shared" si="2"/>
         <v>0.3073593073593075</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>141838.2243776909</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1712,8 +1732,12 @@
         <f t="shared" si="2"/>
         <v>-1.5452538631346657E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>143882.68916712035</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1737,8 +1761,12 @@
         <f t="shared" si="2"/>
         <v>0.85426008968609857</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="M19">
+        <f t="shared" si="3"/>
+        <v>128645.83333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1761,11 +1789,15 @@
         <v>0.13746017296313151</v>
       </c>
       <c r="I20" s="5">
-        <f t="shared" ref="I20" si="3">(C20/C19 - 1)</f>
+        <f t="shared" ref="I20" si="4">(C20/C19 - 1)</f>
         <v>0.13746017296313151</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>120312.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -1788,8 +1820,12 @@
         <v>9.8839535814325918E-2</v>
       </c>
       <c r="I21" s="5">
-        <f t="shared" ref="I21" si="4">(C21/C20 - 1)</f>
+        <f t="shared" ref="I21" si="5">(C21/C20 - 1)</f>
         <v>9.8839535814325918E-2</v>
+      </c>
+      <c r="M21">
+        <f>(E21*15625)/60</f>
+        <v>120312.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UniformPool updates can use dirty ranges (very little performance impact, maybe even none)
</commit_message>
<xml_diff>
--- a/src/TrafoUpdatePerformance.xlsx
+++ b/src/TrafoUpdatePerformance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Initial</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>VolaileCollection using C# List</t>
+  </si>
+  <si>
+    <t>Support for partial updates in UniformBufferPool (id magic)</t>
   </si>
 </sst>
 </file>
@@ -176,9 +179,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Initial</c:v>
                 </c:pt>
@@ -238,16 +241,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>VolaileCollection using C# List</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Support for partial updates in UniformBufferPool (id magic)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:f>Sheet1!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>2.63</c:v>
                 </c:pt>
@@ -307,6 +313,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>27.46</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>28.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -328,9 +337,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Initial</c:v>
                 </c:pt>
@@ -390,16 +399,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>VolaileCollection using C# List</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Support for partial updates in UniformBufferPool (id magic)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$21</c:f>
+              <c:f>Sheet1!$C$2:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>2.1192906976744186</c:v>
                 </c:pt>
@@ -459,29 +471,32 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>20.673117888029132</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.162467000455166</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="71071616"/>
-        <c:axId val="71073152"/>
+        <c:axId val="99714944"/>
+        <c:axId val="99716480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="71071616"/>
+        <c:axId val="99714944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71073152"/>
+        <c:crossAx val="99716480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71073152"/>
+        <c:axId val="99716480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -489,7 +504,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71071616"/>
+        <c:crossAx val="99714944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -502,7 +517,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -533,9 +548,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Initial</c:v>
                 </c:pt>
@@ -595,16 +610,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>VolaileCollection using C# List</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Support for partial updates in UniformBufferPool (id magic)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$21</c:f>
+              <c:f>Sheet1!$H$2:$H$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -664,6 +682,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>9.8839535814325918E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.367079388201021E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -685,9 +706,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>Initial</c:v>
                 </c:pt>
@@ -747,16 +768,19 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>VolaileCollection using C# List</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Support for partial updates in UniformBufferPool (id magic)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$21</c:f>
+              <c:f>Sheet1!$I$2:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -816,29 +840,32 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>9.8839535814325918E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.367079388201021E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="162368128"/>
-        <c:axId val="162578816"/>
+        <c:axId val="100867456"/>
+        <c:axId val="100873344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="162368128"/>
+        <c:axId val="100867456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162578816"/>
+        <c:crossAx val="100873344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162578816"/>
+        <c:axId val="100873344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -847,7 +874,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162368128"/>
+        <c:crossAx val="100867456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -860,7 +887,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1216,15 +1243,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.7109375" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" style="2" customWidth="1"/>
@@ -1325,11 +1352,11 @@
         <v>210.48958333333334</v>
       </c>
       <c r="H4" s="5">
-        <f>(B4/B3 - 1)</f>
+        <f t="shared" ref="H4:H21" si="2">(B4/B3 - 1)</f>
         <v>-3.7453183520598232E-3</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" ref="I4:I19" si="2">(C4/C3 - 1)</f>
+        <f t="shared" ref="I4:I19" si="3">(C4/C3 - 1)</f>
         <v>-3.7453183520599342E-3</v>
       </c>
     </row>
@@ -1352,11 +1379,11 @@
         <v>207.68586208333332</v>
       </c>
       <c r="H5" s="5">
-        <f>(B5/B4 - 1)</f>
+        <f t="shared" si="2"/>
         <v>0.50375939849624052</v>
       </c>
       <c r="I5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.50375939849624052</v>
       </c>
     </row>
@@ -1379,11 +1406,11 @@
         <v>197.43080958333334</v>
       </c>
       <c r="H6" s="5">
-        <f>(B6/B5 - 1)</f>
+        <f t="shared" si="2"/>
         <v>0.1100000000000001</v>
       </c>
       <c r="I6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.1100000000000001</v>
       </c>
     </row>
@@ -1406,11 +1433,11 @@
         <v>197.01824999999999</v>
       </c>
       <c r="H7" s="5">
-        <f>(B7/B6 - 1)</f>
+        <f t="shared" si="2"/>
         <v>0.32432432432432412</v>
       </c>
       <c r="I7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.32432432432432412</v>
       </c>
     </row>
@@ -1433,11 +1460,11 @@
         <v>205.55570749999998</v>
       </c>
       <c r="H8" s="5">
-        <f>(B8/B7 - 1)</f>
+        <f t="shared" si="2"/>
         <v>-6.9727891156462607E-2</v>
       </c>
       <c r="I8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-6.9727891156462496E-2</v>
       </c>
     </row>
@@ -1460,11 +1487,11 @@
         <v>197.01824999999999</v>
       </c>
       <c r="H9" s="5">
-        <f>(B9/B8 - 1)</f>
+        <f t="shared" si="2"/>
         <v>7.6782449725776969E-2</v>
       </c>
       <c r="I9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.6782449725776747E-2</v>
       </c>
     </row>
@@ -1487,11 +1514,11 @@
         <v>207.30698083333334</v>
       </c>
       <c r="H10" s="5">
-        <f>(B10/B9 - 1)</f>
+        <f t="shared" si="2"/>
         <v>1.1884550084889645E-2</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1884550084889645E-2</v>
       </c>
     </row>
@@ -1514,11 +1541,11 @@
         <v>208.51098124999999</v>
       </c>
       <c r="H11" s="5">
-        <f>(B11/B10 - 1)</f>
+        <f t="shared" si="2"/>
         <v>4.8657718120805438E-2</v>
       </c>
       <c r="I11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.865771812080566E-2</v>
       </c>
       <c r="K11" t="s">
@@ -1544,11 +1571,11 @@
         <v>206.27979166666668</v>
       </c>
       <c r="H12" s="5">
-        <f>(B12/B11 - 1)</f>
+        <f t="shared" si="2"/>
         <v>-3.1999999999999806E-3</v>
       </c>
       <c r="I12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.1999999999999806E-3</v>
       </c>
     </row>
@@ -1571,15 +1598,15 @@
         <v>203.4929095833333</v>
       </c>
       <c r="H13" s="5">
-        <f>(B13/B12 - 1)</f>
-        <v>4.6548956661315977E-2</v>
-      </c>
-      <c r="I13" s="5">
         <f t="shared" si="2"/>
         <v>4.6548956661315977E-2</v>
       </c>
+      <c r="I13" s="5">
+        <f t="shared" si="3"/>
+        <v>4.6548956661315977E-2</v>
+      </c>
       <c r="M13">
-        <f t="shared" ref="M13:M20" si="3">(E13*15625)/60</f>
+        <f t="shared" ref="M13:M20" si="4">(E13*15625)/60</f>
         <v>62940.104166666664</v>
       </c>
     </row>
@@ -1602,15 +1629,15 @@
         <v>193.65041666666667</v>
       </c>
       <c r="H14" s="5">
-        <f>(B14/B13 - 1)</f>
-        <v>1.6871165644171793E-2</v>
-      </c>
-      <c r="I14" s="5">
         <f t="shared" si="2"/>
         <v>1.6871165644171793E-2</v>
       </c>
+      <c r="I14" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6871165644171793E-2</v>
+      </c>
       <c r="M14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59895.833333333336</v>
       </c>
     </row>
@@ -1633,15 +1660,15 @@
         <v>202.69304916666667</v>
       </c>
       <c r="H15" s="5">
-        <f>(B15/B14 - 1)</f>
-        <v>0.28205128205128216</v>
-      </c>
-      <c r="I15" s="5">
         <f t="shared" si="2"/>
         <v>0.28205128205128216</v>
       </c>
+      <c r="I15" s="5">
+        <f t="shared" si="3"/>
+        <v>0.28205128205128216</v>
+      </c>
       <c r="M15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>62692.708333333336</v>
       </c>
     </row>
@@ -1662,11 +1689,11 @@
         <v>202.07</v>
       </c>
       <c r="H16" s="5">
-        <f>(B16/B15 - 1)</f>
+        <f t="shared" si="2"/>
         <v>1.1764705882352899E-2</v>
       </c>
       <c r="I16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1764705882352899E-2</v>
       </c>
       <c r="M16">
@@ -1693,15 +1720,15 @@
         <v>458.58</v>
       </c>
       <c r="H17" s="5">
-        <f>(B17/B16 - 1)</f>
-        <v>0.3073593073593075</v>
-      </c>
-      <c r="I17" s="5">
         <f t="shared" si="2"/>
         <v>0.3073593073593075</v>
       </c>
+      <c r="I17" s="5">
+        <f t="shared" si="3"/>
+        <v>0.3073593073593075</v>
+      </c>
       <c r="M17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>141838.2243776909</v>
       </c>
     </row>
@@ -1725,15 +1752,15 @@
         <v>465.19</v>
       </c>
       <c r="H18" s="5">
-        <f>(B18/B17 - 1)</f>
+        <f t="shared" si="2"/>
         <v>-1.5452538631346435E-2</v>
       </c>
       <c r="I18" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1.5452538631346657E-2</v>
       </c>
       <c r="M18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>143882.68916712035</v>
       </c>
     </row>
@@ -1754,15 +1781,15 @@
         <v>468.89</v>
       </c>
       <c r="H19" s="5">
-        <f>(B19/B18 - 1)</f>
+        <f t="shared" si="2"/>
         <v>0.98472338095734657</v>
       </c>
       <c r="I19" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.85426008968609857</v>
       </c>
       <c r="M19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128645.83333333333</v>
       </c>
     </row>
@@ -1785,15 +1812,15 @@
         <v>438.51655870445342</v>
       </c>
       <c r="H20" s="5">
-        <f>(B20/B19 - 1)</f>
+        <f t="shared" si="2"/>
         <v>0.13746017296313151</v>
       </c>
       <c r="I20" s="5">
-        <f t="shared" ref="I20" si="4">(C20/C19 - 1)</f>
+        <f t="shared" ref="I20" si="5">(C20/C19 - 1)</f>
         <v>0.13746017296313151</v>
       </c>
       <c r="M20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>120312.5</v>
       </c>
     </row>
@@ -1816,16 +1843,43 @@
         <v>438.51655870445342</v>
       </c>
       <c r="H21" s="5">
-        <f>(B21/B20 - 1)</f>
+        <f t="shared" si="2"/>
         <v>9.8839535814325918E-2</v>
       </c>
       <c r="I21" s="5">
-        <f t="shared" ref="I21" si="5">(C21/C20 - 1)</f>
+        <f t="shared" ref="I21" si="6">(C21/C20 - 1)</f>
         <v>9.8839535814325918E-2</v>
       </c>
       <c r="M21">
         <f>(E21*15625)/60</f>
         <v>120312.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
+        <v>28.11</v>
+      </c>
+      <c r="C22" s="3">
+        <f>B22*C$19/B$19</f>
+        <v>21.162467000455166</v>
+      </c>
+      <c r="E22" s="2">
+        <v>492.53</v>
+      </c>
+      <c r="F22" s="3">
+        <f>E22*F$19/E$19</f>
+        <v>467.49472004048579</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" ref="H22" si="7">(B22/B21 - 1)</f>
+        <v>2.367079388201021E-2</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" ref="I22" si="8">(C22/C21 - 1)</f>
+        <v>2.367079388201021E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actived new state-trie (wip)
</commit_message>
<xml_diff>
--- a/src/TrafoUpdatePerformance.xlsx
+++ b/src/TrafoUpdatePerformance.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="14385"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="14385" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="TrafoUpdate" sheetId="1" r:id="rId1"/>
+    <sheet name="Compile" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Initial</t>
   </si>
@@ -91,12 +91,18 @@
   </si>
   <si>
     <t>Everything clean again</t>
+  </si>
+  <si>
+    <t>MultiSet for StateTrie (less entries in SortedDictionary)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00&quot; s&quot;"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -139,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -148,6 +154,9 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,7 +168,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
@@ -171,7 +180,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>TrafoUpdate!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -182,7 +191,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$23</c:f>
+              <c:f>TrafoUpdate!$A$2:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
@@ -256,7 +265,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$23</c:f>
+              <c:f>TrafoUpdate!$B$2:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="22"/>
@@ -335,7 +344,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>TrafoUpdate!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -346,7 +355,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$23</c:f>
+              <c:f>TrafoUpdate!$A$2:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
@@ -420,7 +429,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$23</c:f>
+              <c:f>TrafoUpdate!$C$2:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="22"/>
@@ -487,28 +496,31 @@
                 <c:pt idx="20">
                   <c:v>21.162467000455166</c:v>
                 </c:pt>
+                <c:pt idx="21">
+                  <c:v>20.92</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="166434304"/>
-        <c:axId val="166441728"/>
+        <c:axId val="79868288"/>
+        <c:axId val="79869824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166434304"/>
+        <c:axId val="79868288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166441728"/>
+        <c:crossAx val="79869824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166441728"/>
+        <c:axId val="79869824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,7 +528,377 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166434304"/>
+        <c:crossAx val="79868288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TrafoUpdate!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Monster64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>TrafoUpdate!$A$2:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>Initial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>eval depth instead of eval-stack</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>merged depth and locking try-finally</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>no telemetry</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>no List.iter in ChangeableResource UpdateCPU</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>No DirtySet in UniformBuffer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Correct again with Sync (possibly bad)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VolatileSet remains HashSet when consumed</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>no lock in VolatileCollection</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DuplicatePriorityQueue local mutable for outs</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>using null as none-value for current obj in Transaction</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>NativePtr write instead of Marshal.StructureToPtr</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>IWriter</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>optimized update-counting</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>TrafoMultiplyMod</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>UniformBufferView</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>correct again (initial execution)</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>evaluate inline</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>always hashset</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>VolaileCollection using C# List</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Support for partial updates in UniformBufferPool (id magic)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TrafoUpdate!$H$2:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5209125475285079E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.7453183520598232E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50375939849624052</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32432432432432412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-6.9727891156462607E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6782449725776969E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1884550084889645E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8657718120805438E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.1999999999999806E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.6548956661315977E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6871165644171793E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.28205128205128216</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1764705882352899E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3073593073593075</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.5452538631346435E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.98472338095734657</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.13746017296313151</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.8839535814325918E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.367079388201021E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TrafoUpdate!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mobile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>TrafoUpdate!$A$2:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>Initial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>eval depth instead of eval-stack</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>merged depth and locking try-finally</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>no telemetry</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>no List.iter in ChangeableResource UpdateCPU</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>No DirtySet in UniformBuffer</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Correct again with Sync (possibly bad)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VolatileSet remains HashSet when consumed</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>no lock in VolatileCollection</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DuplicatePriorityQueue local mutable for outs</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>using null as none-value for current obj in Transaction</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>NativePtr write instead of Marshal.StructureToPtr</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>IWriter</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>optimized update-counting</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>TrafoMultiplyMod</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>UniformBufferView</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>correct again (initial execution)</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>evaluate inline</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>always hashset</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>VolaileCollection using C# List</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Support for partial updates in UniformBufferPool (id magic)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TrafoUpdate!$I$2:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5209125475285301E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.7453183520599342E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50375939849624052</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32432432432432412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-6.9727891156462496E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6782449725776747E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1884550084889645E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.865771812080566E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-3.1999999999999806E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.6548956661315977E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6871165644171793E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.28205128205128216</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1764705882352899E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3073593073593075</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.5452538631346657E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85426008968609857</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.13746017296313151</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.8839535814325918E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.367079388201021E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="80676736"/>
+        <c:axId val="80678272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="80676736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80678272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="80678272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80676736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -535,10 +917,11 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -549,344 +932,71 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Compile!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Monster64</c:v>
+                  <c:v>Mobile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:f>Compile!$A$2:$A$23</c:f>
               <c:strCache>
-                <c:ptCount val="21"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Initial</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>eval depth instead of eval-stack</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>merged depth and locking try-finally</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>no telemetry</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>no List.iter in ChangeableResource UpdateCPU</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>No DirtySet in UniformBuffer</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Correct again with Sync (possibly bad)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>VolatileSet remains HashSet when consumed</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>no lock in VolatileCollection</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>DuplicatePriorityQueue local mutable for outs</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>using null as none-value for current obj in Transaction</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>NativePtr write instead of Marshal.StructureToPtr</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>IWriter</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>optimized update-counting</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>TrafoMultiplyMod</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>UniformBufferView</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>correct again (initial execution)</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>evaluate inline</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>always hashset</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>VolaileCollection using C# List</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Support for partial updates in UniformBufferPool (id magic)</c:v>
+                  <c:v>MultiSet for StateTrie (less entries in SortedDictionary)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$22</c:f>
+              <c:f>Compile!$C$2:$C$23</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:formatCode>0.00" s"</c:formatCode>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3.64</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5209125475285079E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3.7453183520598232E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.50375939849624052</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1100000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32432432432432412</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-6.9727891156462607E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.6782449725776969E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1884550084889645E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.8657718120805438E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-3.1999999999999806E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.6548956661315977E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6871165644171793E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.28205128205128216</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.1764705882352899E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.3073593073593075</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-1.5452538631346435E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.98472338095734657</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.13746017296313151</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.8839535814325918E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.367079388201021E-2</c:v>
+                  <c:v>2.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mobile</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>Initial</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>eval depth instead of eval-stack</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>merged depth and locking try-finally</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>no telemetry</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>no List.iter in ChangeableResource UpdateCPU</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>No DirtySet in UniformBuffer</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Correct again with Sync (possibly bad)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>VolatileSet remains HashSet when consumed</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>no lock in VolatileCollection</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>DuplicatePriorityQueue local mutable for outs</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>using null as none-value for current obj in Transaction</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>NativePtr write instead of Marshal.StructureToPtr</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>IWriter</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>optimized update-counting</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>TrafoMultiplyMod</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>UniformBufferView</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>correct again (initial execution)</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>evaluate inline</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>always hashset</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>VolaileCollection using C# List</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Support for partial updates in UniformBufferPool (id magic)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$I$2:$I$22</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.5209125475285301E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3.7453183520599342E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.50375939849624052</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1100000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32432432432432412</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-6.9727891156462496E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.6782449725776747E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1884550084889645E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.865771812080566E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-3.1999999999999806E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.6548956661315977E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6871165644171793E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.28205128205128216</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.1764705882352899E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.3073593073593075</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-1.5452538631346657E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.85426008968609857</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.13746017296313151</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.8839535814325918E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.367079388201021E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="53950336"/>
-        <c:axId val="53951872"/>
+        <c:axId val="69279744"/>
+        <c:axId val="69281280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53950336"/>
+        <c:axId val="69279744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53951872"/>
+        <c:crossAx val="69281280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53951872"/>
+        <c:axId val="69281280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00&quot; s&quot;" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53950336"/>
+        <c:crossAx val="69279744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -899,7 +1009,106 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Compile!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mobile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Compile!$A$2:$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Initial</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MultiSet for StateTrie (less entries in SortedDictionary)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Compile!$H$2:$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35315985130111538</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="69428736"/>
+        <c:axId val="69430272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="69428736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69430272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69430272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69428736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -910,15 +1119,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>742949</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>723899</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -953,6 +1162,71 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723899</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>723899</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1257,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1901,6 +2175,23 @@
       <c r="B23" s="2">
         <v>25</v>
       </c>
+      <c r="C23" s="2">
+        <v>20.92</v>
+      </c>
+      <c r="E23" s="2">
+        <v>493.23</v>
+      </c>
+      <c r="F23" s="2">
+        <v>469.51</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" ref="H23" si="9">(B23/B22 - 1)</f>
+        <v>-0.11063678406261113</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" ref="I23" si="10">(C23/C22 - 1)</f>
+        <v>-1.1457407137360209E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1911,13 +2202,216 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="58.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="5" customWidth="1"/>
+    <col min="10" max="22" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7">
+        <v>3.64</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7">
+        <v>2.69</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="H3" s="5">
+        <f>(C2/C3)-1</f>
+        <v>0.35315985130111538</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="3"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="3"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="5"/>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="3"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1"/>
+      <c r="B18" s="8"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1"/>
+      <c r="B19" s="7"/>
+      <c r="E19" s="4"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1"/>
+      <c r="C20" s="8"/>
+      <c r="F20" s="3"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1"/>
+      <c r="C21" s="8"/>
+      <c r="F21" s="3"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1"/>
+      <c r="C22" s="8"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1"/>
+      <c r="H23" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>